<commit_message>
arumando erros como numeros que não existem
</commit_message>
<xml_diff>
--- a/planilhas/andreynumeros.xlsx
+++ b/planilhas/andreynumeros.xlsx
@@ -445,18 +445,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>4898418335</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-    </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
@@ -465,7 +453,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>1.0</t>
         </is>
       </c>
     </row>

</xml_diff>